<commit_message>
Puliendo la estructura de los data frames de CPU y MEM
</commit_message>
<xml_diff>
--- a/procesosCPU.xlsx
+++ b/procesosCPU.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="procesosMEM" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="procesosCPU" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -462,16 +462,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8151</v>
+        <v>29</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.07%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.04%</t>
+          <t>0.00%</t>
         </is>
       </c>
     </row>
@@ -482,16 +482,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8151</v>
+        <v>29</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>9.37%</t>
+          <t>0.26%</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.35%</t>
+          <t>0.06%</t>
         </is>
       </c>
     </row>
@@ -502,16 +502,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8097</v>
+        <v>29</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.88%</t>
+          <t>0.04%</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.06%</t>
+          <t>0.00%</t>
         </is>
       </c>
     </row>
@@ -522,16 +522,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8055</v>
+        <v>29</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.45%</t>
+          <t>0.04%</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.20%</t>
+          <t>0.00%</t>
         </is>
       </c>
     </row>
@@ -542,16 +542,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>8055</v>
+        <v>29</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>9.05%</t>
+          <t>0.04%</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.89%</t>
+          <t>0.00%</t>
         </is>
       </c>
     </row>
@@ -562,16 +562,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8055</v>
+        <v>29</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.17%</t>
+          <t>0.05%</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.09%</t>
+          <t>0.00%</t>
         </is>
       </c>
     </row>
@@ -582,16 +582,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>8055</v>
+        <v>29</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>9.98%</t>
+          <t>0.06%</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.96%</t>
+          <t>0.00%</t>
         </is>
       </c>
     </row>
@@ -602,16 +602,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8148</v>
+        <v>29</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2.65%</t>
+          <t>0.09%</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.55%</t>
+          <t>0.00%</t>
         </is>
       </c>
     </row>
@@ -622,16 +622,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8100</v>
+        <v>29</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.60%</t>
+          <t>35.40%</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0.22%</t>
         </is>
       </c>
     </row>
@@ -642,16 +642,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>8148</v>
+        <v>29</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.11%</t>
+          <t>0.30%</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.06%</t>
+          <t>0.22%</t>
         </is>
       </c>
     </row>
@@ -662,16 +662,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>8150</v>
+        <v>29</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>7.00%</t>
+          <t>1.06%</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.69%</t>
+          <t>0.67%</t>
         </is>
       </c>
     </row>
@@ -682,16 +682,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>176</v>
+        <v>29</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>3.64%</t>
+          <t>3.42%</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3.63%</t>
+          <t>0.69%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Puliendo estuctura del codigo
</commit_message>
<xml_diff>
--- a/procesosCPU.xlsx
+++ b/procesosCPU.xlsx
@@ -462,11 +462,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>29</v>
+        <v>8151</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>1.73%</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -482,16 +482,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>29</v>
+        <v>8151</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.26%</t>
+          <t>9.15%</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.06%</t>
+          <t>0.03%</t>
         </is>
       </c>
     </row>
@@ -502,11 +502,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>29</v>
+        <v>8097</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.04%</t>
+          <t>9.98%</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -522,11 +522,11 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>29</v>
+        <v>8055</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.04%</t>
+          <t>99.90%</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -542,11 +542,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>29</v>
+        <v>8055</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.04%</t>
+          <t>99.76%</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -562,11 +562,11 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>29</v>
+        <v>8055</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.05%</t>
+          <t>2.50%</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -582,11 +582,11 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>29</v>
+        <v>8055</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.06%</t>
+          <t>99.98%</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -602,11 +602,11 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>29</v>
+        <v>8148</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.09%</t>
+          <t>9.99%</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -622,16 +622,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>29</v>
+        <v>8100</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>35.40%</t>
+          <t>94.87%</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.22%</t>
+          <t>0.00%</t>
         </is>
       </c>
     </row>
@@ -642,16 +642,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>29</v>
+        <v>8148</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.30%</t>
+          <t>9.86%</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.22%</t>
+          <t>0.12%</t>
         </is>
       </c>
     </row>
@@ -662,16 +662,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>29</v>
+        <v>8150</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.06%</t>
+          <t>9.82%</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.67%</t>
+          <t>0.27%</t>
         </is>
       </c>
     </row>
@@ -682,16 +682,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>29</v>
+        <v>176</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>3.42%</t>
+          <t>3.79%</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.69%</t>
+          <t>0.54%</t>
         </is>
       </c>
     </row>

</xml_diff>